<commit_message>
Updated Head of table
</commit_message>
<xml_diff>
--- a/province_numbers.xlsx
+++ b/province_numbers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\4. FS\Data analysis\Extracted Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/niklas_winata_bwedu_de/Documents/Dokumente/GitHub/topic04_team02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E31823F-E476-4655-84C4-4897C8CF4342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{6E31823F-E476-4655-84C4-4897C8CF4342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43972F8C-725D-449B-9D99-3E4938B50421}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8FC4C610-D24A-43A5-8AD8-320000C50D5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t>TH-10</t>
   </si>
@@ -498,6 +498,15 @@
   </si>
   <si>
     <t>Bangkok</t>
+  </si>
+  <si>
+    <t>ISO Code</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
 </sst>
 </file>
@@ -533,9 +542,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -852,865 +860,873 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C4EF3E-A3FF-4472-B44B-61996D83F17C}">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>153</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" t="s">
         <v>38</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" t="s">
         <v>42</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" t="s">
         <v>44</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" t="s">
         <v>50</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" t="s">
         <v>52</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" t="s">
         <v>54</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" t="s">
         <v>56</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" t="s">
         <v>58</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" t="s">
         <v>60</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" t="s">
         <v>62</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" t="s">
         <v>66</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" t="s">
         <v>68</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" t="s">
         <v>70</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" t="s">
         <v>74</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" t="s">
         <v>76</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" t="s">
         <v>78</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" t="s">
         <v>80</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" t="s">
         <v>82</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" t="s">
         <v>84</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" t="s">
         <v>86</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" t="s">
         <v>88</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" t="s">
         <v>90</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" t="s">
         <v>92</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" t="s">
         <v>94</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" t="s">
         <v>96</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" t="s">
         <v>98</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" t="s">
         <v>100</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" t="s">
         <v>102</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>103</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" t="s">
         <v>104</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" t="s">
         <v>106</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" t="s">
         <v>108</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" t="s">
         <v>110</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" t="s">
         <v>112</v>
       </c>
-      <c r="C57">
+      <c r="C58">
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" t="s">
         <v>114</v>
       </c>
-      <c r="C58">
+      <c r="C59">
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>115</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" t="s">
         <v>116</v>
       </c>
-      <c r="C59">
+      <c r="C60">
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" t="s">
         <v>118</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>119</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" t="s">
         <v>120</v>
       </c>
-      <c r="C61">
+      <c r="C62">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" t="s">
         <v>122</v>
       </c>
-      <c r="C62">
+      <c r="C63">
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" t="s">
         <v>124</v>
       </c>
-      <c r="C63">
+      <c r="C64">
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" t="s">
         <v>126</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" t="s">
         <v>128</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <v>81</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" t="s">
         <v>130</v>
       </c>
-      <c r="C66">
+      <c r="C67">
         <v>82</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>131</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" t="s">
         <v>132</v>
       </c>
-      <c r="C67">
+      <c r="C68">
         <v>83</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>133</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" t="s">
         <v>134</v>
       </c>
-      <c r="C68">
+      <c r="C69">
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" t="s">
         <v>136</v>
       </c>
-      <c r="C69">
+      <c r="C70">
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" t="s">
         <v>138</v>
       </c>
-      <c r="C70">
+      <c r="C71">
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" t="s">
         <v>140</v>
       </c>
-      <c r="C71">
+      <c r="C72">
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" t="s">
         <v>142</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>143</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" t="s">
         <v>144</v>
       </c>
-      <c r="C73">
+      <c r="C74">
         <v>92</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>145</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" t="s">
         <v>146</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>93</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" t="s">
         <v>148</v>
       </c>
-      <c r="C75">
+      <c r="C76">
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>149</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" t="s">
         <v>150</v>
       </c>
-      <c r="C76">
+      <c r="C77">
         <v>95</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>151</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" t="s">
         <v>152</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>96</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>